<commit_message>
more audit baruch hashem
</commit_message>
<xml_diff>
--- a/childsmile/childsmile_app/1.xlsx
+++ b/childsmile/childsmile_app/1.xlsx
@@ -14,32 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>description</t>
   </si>
   <si>
     <t>User: שלמה_בונצל
 Email: shlezi0@gmail.com
-Action: Failed update staff
-Staff name: Unknown
-Staff email: Unknown
-Attempted changes: 0 field(s)
-Error: Invalid code
-Admin roles: System Administrator
-Record ID: 121</t>
+Action: Updated task
+Task type: ראיון מועמד לחונכות
+Changes: 1 field(s)
+  • Status: 'הושלמה' → 'בביצוע'
+Roles: System Administrator
+Record ID: 189</t>
   </si>
   <si>
     <t>User: שלמה_בונצל
 Email: shlezi0@gmail.com
-Action: Updated staff member
-Staff name: גדגכדג3 דגכדגכ
-Staff email: asd@asdasd.asdasd
+Action: Deleted pending tutor
+Volunteer: בהככ כדגד
+Reason: Promoted to Tutor
+Task ID: 189
+Status: Successfully promoted
+Roles: System Administrator</t>
+  </si>
+  <si>
+    <t>User: שלמה_בונצל
+Email: shlezi0@gmail.com
+Action: Updated task
+Task type: ראיון מועמד לחונכות
 Changes: 1 field(s)
-  • First Name: 'גדגכדג' → 'גדגכדג3'
-Assigned roles: Tutor
-Admin roles: System Administrator
-Record ID: 121</t>
+  • Status: 'בביצוע' → 'לא הושלמה'
+Roles: System Administrator
+Record ID: 189</t>
   </si>
 </sst>
 </file>
@@ -380,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,6 +408,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>